<commit_message>
update datamodel and mvp config example
</commit_message>
<xml_diff>
--- a/doc/assets/example_assets.xlsx
+++ b/doc/assets/example_assets.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,16 +462,6 @@
           <t>eta_r</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>deliveryTemp_degc</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>capacityHeat_kW</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,28 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GAS_BURNER</t>
+          <t>DIESEL_VEHICLE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ChemicalHeatConversionAsset</t>
+          <t>VehicleConversionAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Building_gas_burner_60kW</t>
+          <t>Diesel_Truck</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>0.95</v>
       </c>
-      <c r="F2" t="n">
-        <v>90</v>
-      </c>
-      <c r="G2" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,11 +512,30 @@
       <c r="E3" t="n">
         <v>0.95</v>
       </c>
-      <c r="F3" t="n">
-        <v>90</v>
-      </c>
-      <c r="G3" t="n">
-        <v>60</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CONVERSION</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GAS_BURNER</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ChemicalHeatConversionAsset</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Building_gas_burner_60kW</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +580,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>yearlyDemandElectricity_kWh</t>
+          <t>yearlyDemandHeat_kWh</t>
         </is>
       </c>
     </row>
@@ -589,21 +592,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTRICITY_DEMAND</t>
+          <t>HEAT_DEMAND</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ElectricConsumptionAsset</t>
+          <t>HeatConsumptionAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Logistics_fleet_hgv_E</t>
+          <t>INDUSTRY_OTHER_HEAT_DEMAND</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6500000</v>
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -695,11 +698,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Building_solarpanels_0kWp</t>
+          <t>Building_solarpanels_10kWp</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -720,11 +723,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Solarpanels_1MW</t>
+          <t>Building_solarpanels_0kWp</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -749,6 +752,31 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PRODUCTION</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PHOTOVOLTAIC</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ElectricProductionAsset</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Solarpanels_1MW</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -763,7 +791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -789,17 +817,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>stateOfCharge_r</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>capacityElectricity_kW</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>stateOfCharge_r</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -816,26 +844,243 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>VehicleElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>EHGV</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>STORAGE_ELECTRIC</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>ElectricStorageAsset</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Grid_battery_7MWh</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>STORAGE_ELECTRIC</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ElectricStorageAsset</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Grid_battery_10MWh</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F9" t="n">
         <v>2000</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="G9" t="n">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to working version!
</commit_message>
<xml_diff>
--- a/doc/assets/example_assets.xlsx
+++ b/doc/assets/example_assets.xlsx
@@ -844,7 +844,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -999,7 +999,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+          <t>ELECTRIC_VEHICLE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">

</xml_diff>